<commit_message>
added color support and fixed bug wih list merger in data_processor
</commit_message>
<xml_diff>
--- a/input/molecule_info/Particulate_List.xlsx
+++ b/input/molecule_info/Particulate_List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11500" yWindow="460" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="46520" yWindow="5360" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Particulates" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="35">
   <si>
     <t>Particulate</t>
   </si>
@@ -37,16 +37,119 @@
   </si>
   <si>
     <t>jager_mgsio3.nc</t>
+  </si>
+  <si>
+    <t>Common Name</t>
+  </si>
+  <si>
+    <t>Feyalite</t>
+  </si>
+  <si>
+    <t>jena_fe2sio4.nc</t>
+  </si>
+  <si>
+    <t>fe2sio4</t>
+  </si>
+  <si>
+    <t>tholins</t>
+  </si>
+  <si>
+    <t>khare_tholins.nc</t>
+  </si>
+  <si>
+    <t>Mix_1</t>
+  </si>
+  <si>
+    <t>afcrl1987_shettle.nc</t>
+  </si>
+  <si>
+    <t>feo</t>
+  </si>
+  <si>
+    <t>henning_feo.nc</t>
+  </si>
+  <si>
+    <t>mg2sio4</t>
+  </si>
+  <si>
+    <t>jager_mg2sio4.nc</t>
+  </si>
+  <si>
+    <t>soot</t>
+  </si>
+  <si>
+    <t>querry_diesel_soot.nc</t>
+  </si>
+  <si>
+    <t>zns</t>
+  </si>
+  <si>
+    <t>querry_zns.nc</t>
+  </si>
+  <si>
+    <t>Titan_Aerosol</t>
+  </si>
+  <si>
+    <t>Mix_2</t>
+  </si>
+  <si>
+    <t>ramirez_titan_aerosol.nc</t>
+  </si>
+  <si>
+    <t>Mix_3</t>
+  </si>
+  <si>
+    <t>sinyuk_saharan_dust.nc</t>
+  </si>
+  <si>
+    <t>Mix_4</t>
+  </si>
+  <si>
+    <t>wagner_sahara_dust.nc</t>
+  </si>
+  <si>
+    <t>sio2</t>
+  </si>
+  <si>
+    <t>zeidler_sio2_928k_ab.nc</t>
+  </si>
+  <si>
+    <t>al2o3</t>
+  </si>
+  <si>
+    <t>begemann_al2o3_compact.nc</t>
+  </si>
+  <si>
+    <t>begemann_al2o3_porous.nc</t>
+  </si>
+  <si>
+    <t>Refractive_Info</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -69,13 +172,69 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="29">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -405,168 +564,291 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
       <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="B16" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2">
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2">
-      <c r="B20" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2">
-      <c r="B21" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2">
-      <c r="B22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2">
-      <c r="B23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2">
-      <c r="B24" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2">
-      <c r="B25" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2">
-      <c r="B26" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="C22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="C23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="C25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>23</v>
+      </c>
       <c r="B27" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2">
-      <c r="B28" t="s">
-        <v>3</v>
+        <v>22</v>
+      </c>
+      <c r="C27" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="C30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="C31" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="C32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3">
+      <c r="C33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3">
+      <c r="C34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3">
+      <c r="C36" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>